<commit_message>
- fixes in connectivity and autoreconnect - passive mode is now default
</commit_message>
<xml_diff>
--- a/data/sheet/msg_41473.xlsx
+++ b/data/sheet/msg_41473.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2041" uniqueCount="158">
   <si>
     <t/>
   </si>
@@ -440,6 +440,63 @@
   <si>
     <t>2022-03-18 15:23:00</t>
   </si>
+  <si>
+    <t>2022-03-20 07:29:34</t>
+  </si>
+  <si>
+    <t>2022-03-20 07:36:32</t>
+  </si>
+  <si>
+    <t>2022-03-20 07:39:44</t>
+  </si>
+  <si>
+    <t>2022-03-20 07:46:57</t>
+  </si>
+  <si>
+    <t>2022-03-20 07:49:05</t>
+  </si>
+  <si>
+    <t>2022-03-20 07:50:11</t>
+  </si>
+  <si>
+    <t>2022-03-20 07:52:20</t>
+  </si>
+  <si>
+    <t>2022-03-20 07:53:04</t>
+  </si>
+  <si>
+    <t>2022-03-20 08:23:27</t>
+  </si>
+  <si>
+    <t>2022-03-20 09:19:43</t>
+  </si>
+  <si>
+    <t>2022-03-21 09:32:55</t>
+  </si>
+  <si>
+    <t>2022-03-21 09:34:40</t>
+  </si>
+  <si>
+    <t>2022-03-21 09:38:57</t>
+  </si>
+  <si>
+    <t>2022-03-21 09:57:59</t>
+  </si>
+  <si>
+    <t>2022-03-21 09:59:22</t>
+  </si>
+  <si>
+    <t>2022-03-21 10:01:21</t>
+  </si>
+  <si>
+    <t>2022-03-21 10:02:12</t>
+  </si>
+  <si>
+    <t>2022-03-21 10:03:17</t>
+  </si>
+  <si>
+    <t>2022-03-21 10:55:46</t>
+  </si>
 </sst>
 </file>
 
@@ -791,7 +848,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I114"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3557,6 +3614,557 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>139</v>
+      </c>
+      <c r="B96" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" t="n">
+        <v>1.647757774E9</v>
+      </c>
+      <c r="E96" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F96" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G96" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I96" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>140</v>
+      </c>
+      <c r="B97" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" t="n">
+        <v>1.647758192E9</v>
+      </c>
+      <c r="E97" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F97" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G97" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I97" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>141</v>
+      </c>
+      <c r="B98" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D98" t="n">
+        <v>1.647758384E9</v>
+      </c>
+      <c r="E98" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G98" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I98" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>142</v>
+      </c>
+      <c r="B99" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" t="n">
+        <v>1.647758817E9</v>
+      </c>
+      <c r="E99" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I99" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>143</v>
+      </c>
+      <c r="B100" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" t="n">
+        <v>1.647758944E9</v>
+      </c>
+      <c r="E100" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F100" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G100" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I100" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>144</v>
+      </c>
+      <c r="B101" t="s">
+        <v>0</v>
+      </c>
+      <c r="C101" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" t="n">
+        <v>1.647759011E9</v>
+      </c>
+      <c r="E101" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F101" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G101" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I101" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>145</v>
+      </c>
+      <c r="B102" t="s">
+        <v>0</v>
+      </c>
+      <c r="C102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" t="n">
+        <v>1.64775914E9</v>
+      </c>
+      <c r="E102" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F102" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G102" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I102" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>146</v>
+      </c>
+      <c r="B103" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" t="n">
+        <v>1.647759184E9</v>
+      </c>
+      <c r="E103" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F103" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G103" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I103" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>147</v>
+      </c>
+      <c r="B104" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" t="s">
+        <v>11</v>
+      </c>
+      <c r="D104" t="n">
+        <v>1.647761007E9</v>
+      </c>
+      <c r="E104" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F104" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G104" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I104" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>148</v>
+      </c>
+      <c r="B105" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105" t="n">
+        <v>1.647764383E9</v>
+      </c>
+      <c r="E105" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F105" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G105" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I105" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>149</v>
+      </c>
+      <c r="B106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" t="n">
+        <v>1.647851576E9</v>
+      </c>
+      <c r="E106" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F106" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G106" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I106" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>150</v>
+      </c>
+      <c r="B107" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" t="s">
+        <v>11</v>
+      </c>
+      <c r="D107" t="n">
+        <v>1.647851681E9</v>
+      </c>
+      <c r="E107" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F107" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G107" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I107" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>151</v>
+      </c>
+      <c r="B108" t="s">
+        <v>0</v>
+      </c>
+      <c r="C108" t="s">
+        <v>11</v>
+      </c>
+      <c r="D108" t="n">
+        <v>1.647851938E9</v>
+      </c>
+      <c r="E108" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F108" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G108" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I108" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>152</v>
+      </c>
+      <c r="B109" t="s">
+        <v>0</v>
+      </c>
+      <c r="C109" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109" t="n">
+        <v>1.64785308E9</v>
+      </c>
+      <c r="E109" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F109" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G109" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I109" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>153</v>
+      </c>
+      <c r="B110" t="s">
+        <v>0</v>
+      </c>
+      <c r="C110" t="s">
+        <v>11</v>
+      </c>
+      <c r="D110" t="n">
+        <v>1.647853163E9</v>
+      </c>
+      <c r="E110" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F110" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G110" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I110" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>154</v>
+      </c>
+      <c r="B111" t="s">
+        <v>0</v>
+      </c>
+      <c r="C111" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" t="n">
+        <v>1.647853282E9</v>
+      </c>
+      <c r="E111" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F111" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G111" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I111" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>155</v>
+      </c>
+      <c r="B112" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" t="s">
+        <v>11</v>
+      </c>
+      <c r="D112" t="n">
+        <v>1.647853333E9</v>
+      </c>
+      <c r="E112" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F112" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G112" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I112" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>156</v>
+      </c>
+      <c r="B113" t="s">
+        <v>0</v>
+      </c>
+      <c r="C113" t="s">
+        <v>11</v>
+      </c>
+      <c r="D113" t="n">
+        <v>1.647853398E9</v>
+      </c>
+      <c r="E113" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F113" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G113" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I113" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>157</v>
+      </c>
+      <c r="B114" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" t="n">
+        <v>1.647856548E9</v>
+      </c>
+      <c r="E114" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F114" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G114" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I114" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3564,7 +4172,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X95"/>
+  <dimension ref="A1:X114"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0"/>
   </sheetViews>
@@ -10605,6 +11213,1412 @@
         <v>0</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>139</v>
+      </c>
+      <c r="B96" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D96" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E96" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I96" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J96" t="n">
+        <v>1.647757773E9</v>
+      </c>
+      <c r="K96" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="L96" t="s">
+        <v>0</v>
+      </c>
+      <c r="M96" t="s">
+        <v>0</v>
+      </c>
+      <c r="N96" t="s">
+        <v>0</v>
+      </c>
+      <c r="O96" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X96" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>140</v>
+      </c>
+      <c r="B97" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D97" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E97" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I97" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J97" t="n">
+        <v>1.647758191E9</v>
+      </c>
+      <c r="K97" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="L97" t="s">
+        <v>0</v>
+      </c>
+      <c r="M97" t="s">
+        <v>0</v>
+      </c>
+      <c r="N97" t="s">
+        <v>0</v>
+      </c>
+      <c r="O97" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X97" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>141</v>
+      </c>
+      <c r="B98" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D98" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E98" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G98" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H98" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I98" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J98" t="n">
+        <v>1.647758383E9</v>
+      </c>
+      <c r="K98" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="L98" t="s">
+        <v>0</v>
+      </c>
+      <c r="M98" t="s">
+        <v>0</v>
+      </c>
+      <c r="N98" t="s">
+        <v>0</v>
+      </c>
+      <c r="O98" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X98" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>142</v>
+      </c>
+      <c r="B99" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D99" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E99" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H99" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I99" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J99" t="n">
+        <v>1.647758817E9</v>
+      </c>
+      <c r="K99" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="L99" t="s">
+        <v>0</v>
+      </c>
+      <c r="M99" t="s">
+        <v>0</v>
+      </c>
+      <c r="N99" t="s">
+        <v>0</v>
+      </c>
+      <c r="O99" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X99" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>143</v>
+      </c>
+      <c r="B100" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D100" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E100" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G100" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H100" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I100" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J100" t="n">
+        <v>1.647758944E9</v>
+      </c>
+      <c r="K100" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="L100" t="s">
+        <v>0</v>
+      </c>
+      <c r="M100" t="s">
+        <v>0</v>
+      </c>
+      <c r="N100" t="s">
+        <v>0</v>
+      </c>
+      <c r="O100" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X100" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>144</v>
+      </c>
+      <c r="B101" t="s">
+        <v>0</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D101" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E101" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G101" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H101" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I101" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J101" t="n">
+        <v>1.647759011E9</v>
+      </c>
+      <c r="K101" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="L101" t="s">
+        <v>0</v>
+      </c>
+      <c r="M101" t="s">
+        <v>0</v>
+      </c>
+      <c r="N101" t="s">
+        <v>0</v>
+      </c>
+      <c r="O101" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X101" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>145</v>
+      </c>
+      <c r="B102" t="s">
+        <v>0</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D102" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E102" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I102" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J102" t="n">
+        <v>1.64775914E9</v>
+      </c>
+      <c r="K102" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="L102" t="s">
+        <v>0</v>
+      </c>
+      <c r="M102" t="s">
+        <v>0</v>
+      </c>
+      <c r="N102" t="s">
+        <v>0</v>
+      </c>
+      <c r="O102" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X102" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>146</v>
+      </c>
+      <c r="B103" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D103" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E103" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I103" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J103" t="n">
+        <v>1.64775914E9</v>
+      </c>
+      <c r="K103" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="L103" t="s">
+        <v>0</v>
+      </c>
+      <c r="M103" t="s">
+        <v>0</v>
+      </c>
+      <c r="N103" t="s">
+        <v>0</v>
+      </c>
+      <c r="O103" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X103" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>147</v>
+      </c>
+      <c r="B104" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D104" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E104" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G104" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H104" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I104" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J104" t="n">
+        <v>1.647761007E9</v>
+      </c>
+      <c r="K104" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="L104" t="s">
+        <v>0</v>
+      </c>
+      <c r="M104" t="s">
+        <v>0</v>
+      </c>
+      <c r="N104" t="s">
+        <v>0</v>
+      </c>
+      <c r="O104" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X104" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>148</v>
+      </c>
+      <c r="B105" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D105" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E105" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G105" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H105" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I105" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J105" t="n">
+        <v>1.647764382E9</v>
+      </c>
+      <c r="K105" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="L105" t="s">
+        <v>0</v>
+      </c>
+      <c r="M105" t="s">
+        <v>0</v>
+      </c>
+      <c r="N105" t="s">
+        <v>0</v>
+      </c>
+      <c r="O105" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X105" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>149</v>
+      </c>
+      <c r="B106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D106" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E106" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G106" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H106" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I106" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J106" t="n">
+        <v>1.647851575E9</v>
+      </c>
+      <c r="K106" t="n">
+        <v>68.0</v>
+      </c>
+      <c r="L106" t="s">
+        <v>0</v>
+      </c>
+      <c r="M106" t="s">
+        <v>45</v>
+      </c>
+      <c r="N106" t="s">
+        <v>0</v>
+      </c>
+      <c r="O106" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X106" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>150</v>
+      </c>
+      <c r="B107" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D107" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E107" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G107" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H107" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I107" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J107" t="n">
+        <v>1.647851681E9</v>
+      </c>
+      <c r="K107" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="L107" t="s">
+        <v>0</v>
+      </c>
+      <c r="M107" t="s">
+        <v>0</v>
+      </c>
+      <c r="N107" t="s">
+        <v>0</v>
+      </c>
+      <c r="O107" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X107" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>151</v>
+      </c>
+      <c r="B108" t="s">
+        <v>0</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D108" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E108" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G108" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H108" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I108" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J108" t="n">
+        <v>1.647851937E9</v>
+      </c>
+      <c r="K108" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="L108" t="s">
+        <v>0</v>
+      </c>
+      <c r="M108" t="s">
+        <v>0</v>
+      </c>
+      <c r="N108" t="s">
+        <v>0</v>
+      </c>
+      <c r="O108" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X108" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>152</v>
+      </c>
+      <c r="B109" t="s">
+        <v>0</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D109" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E109" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I109" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J109" t="n">
+        <v>1.647853079E9</v>
+      </c>
+      <c r="K109" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="L109" t="s">
+        <v>0</v>
+      </c>
+      <c r="M109" t="s">
+        <v>0</v>
+      </c>
+      <c r="N109" t="s">
+        <v>0</v>
+      </c>
+      <c r="O109" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X109" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>153</v>
+      </c>
+      <c r="B110" t="s">
+        <v>0</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D110" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E110" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G110" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H110" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I110" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J110" t="n">
+        <v>1.647853162E9</v>
+      </c>
+      <c r="K110" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="L110" t="s">
+        <v>0</v>
+      </c>
+      <c r="M110" t="s">
+        <v>0</v>
+      </c>
+      <c r="N110" t="s">
+        <v>0</v>
+      </c>
+      <c r="O110" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X110" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>154</v>
+      </c>
+      <c r="B111" t="s">
+        <v>0</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D111" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E111" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I111" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J111" t="n">
+        <v>1.647853282E9</v>
+      </c>
+      <c r="K111" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="L111" t="s">
+        <v>0</v>
+      </c>
+      <c r="M111" t="s">
+        <v>0</v>
+      </c>
+      <c r="N111" t="s">
+        <v>0</v>
+      </c>
+      <c r="O111" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X111" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>155</v>
+      </c>
+      <c r="B112" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D112" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E112" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I112" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J112" t="n">
+        <v>1.647853282E9</v>
+      </c>
+      <c r="K112" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="L112" t="s">
+        <v>0</v>
+      </c>
+      <c r="M112" t="s">
+        <v>0</v>
+      </c>
+      <c r="N112" t="s">
+        <v>0</v>
+      </c>
+      <c r="O112" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X112" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>156</v>
+      </c>
+      <c r="B113" t="s">
+        <v>0</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D113" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E113" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I113" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J113" t="n">
+        <v>1.647853398E9</v>
+      </c>
+      <c r="K113" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="L113" t="s">
+        <v>0</v>
+      </c>
+      <c r="M113" t="s">
+        <v>0</v>
+      </c>
+      <c r="N113" t="s">
+        <v>0</v>
+      </c>
+      <c r="O113" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X113" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>157</v>
+      </c>
+      <c r="B114" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D114" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E114" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G114" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H114" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I114" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J114" t="n">
+        <v>1.647856547E9</v>
+      </c>
+      <c r="K114" t="n">
+        <v>68.0</v>
+      </c>
+      <c r="L114" t="s">
+        <v>0</v>
+      </c>
+      <c r="M114" t="s">
+        <v>0</v>
+      </c>
+      <c r="N114" t="s">
+        <v>0</v>
+      </c>
+      <c r="O114" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X114" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10612,7 +12626,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M283"/>
+  <dimension ref="A1:M340"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A278" sqref="A278:XFD280"/>
@@ -22227,6 +24241,2343 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="284">
+      <c r="A284" t="s">
+        <v>139</v>
+      </c>
+      <c r="B284" t="s">
+        <v>0</v>
+      </c>
+      <c r="C284" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D284" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E284" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F284" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G284" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H284" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I284" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J284" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K284" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L284" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M284" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s">
+        <v>139</v>
+      </c>
+      <c r="B285" t="s">
+        <v>0</v>
+      </c>
+      <c r="C285" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D285" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E285" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F285" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G285" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H285" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I285" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J285" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K285" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L285" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M285" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s">
+        <v>139</v>
+      </c>
+      <c r="B286" t="s">
+        <v>0</v>
+      </c>
+      <c r="C286" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D286" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E286" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F286" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G286" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H286" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I286" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J286" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K286" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L286" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M286" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s">
+        <v>140</v>
+      </c>
+      <c r="B287" t="s">
+        <v>0</v>
+      </c>
+      <c r="C287" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D287" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E287" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F287" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G287" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H287" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I287" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J287" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K287" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L287" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M287" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="s">
+        <v>140</v>
+      </c>
+      <c r="B288" t="s">
+        <v>0</v>
+      </c>
+      <c r="C288" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D288" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E288" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F288" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G288" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H288" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I288" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J288" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K288" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L288" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M288" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="s">
+        <v>140</v>
+      </c>
+      <c r="B289" t="s">
+        <v>0</v>
+      </c>
+      <c r="C289" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D289" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E289" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F289" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G289" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H289" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I289" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J289" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K289" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L289" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M289" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="s">
+        <v>141</v>
+      </c>
+      <c r="B290" t="s">
+        <v>0</v>
+      </c>
+      <c r="C290" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D290" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E290" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F290" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G290" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H290" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I290" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J290" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K290" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L290" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M290" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="s">
+        <v>141</v>
+      </c>
+      <c r="B291" t="s">
+        <v>0</v>
+      </c>
+      <c r="C291" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D291" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E291" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F291" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G291" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H291" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I291" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J291" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K291" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L291" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M291" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s">
+        <v>141</v>
+      </c>
+      <c r="B292" t="s">
+        <v>0</v>
+      </c>
+      <c r="C292" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D292" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E292" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F292" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G292" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H292" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I292" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J292" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K292" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L292" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M292" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s">
+        <v>142</v>
+      </c>
+      <c r="B293" t="s">
+        <v>0</v>
+      </c>
+      <c r="C293" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D293" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E293" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F293" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G293" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H293" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I293" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J293" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K293" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L293" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M293" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s">
+        <v>142</v>
+      </c>
+      <c r="B294" t="s">
+        <v>0</v>
+      </c>
+      <c r="C294" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D294" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E294" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F294" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G294" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H294" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I294" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J294" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K294" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L294" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M294" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s">
+        <v>142</v>
+      </c>
+      <c r="B295" t="s">
+        <v>0</v>
+      </c>
+      <c r="C295" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D295" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E295" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F295" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G295" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H295" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I295" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J295" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K295" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L295" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M295" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s">
+        <v>143</v>
+      </c>
+      <c r="B296" t="s">
+        <v>0</v>
+      </c>
+      <c r="C296" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D296" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E296" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F296" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G296" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H296" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I296" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J296" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K296" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L296" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M296" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s">
+        <v>143</v>
+      </c>
+      <c r="B297" t="s">
+        <v>0</v>
+      </c>
+      <c r="C297" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D297" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E297" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F297" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G297" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H297" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I297" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J297" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K297" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L297" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M297" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s">
+        <v>143</v>
+      </c>
+      <c r="B298" t="s">
+        <v>0</v>
+      </c>
+      <c r="C298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D298" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F298" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G298" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H298" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I298" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J298" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M298" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s">
+        <v>144</v>
+      </c>
+      <c r="B299" t="s">
+        <v>0</v>
+      </c>
+      <c r="C299" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D299" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E299" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F299" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G299" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H299" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I299" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J299" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K299" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L299" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M299" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s">
+        <v>144</v>
+      </c>
+      <c r="B300" t="s">
+        <v>0</v>
+      </c>
+      <c r="C300" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D300" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E300" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F300" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G300" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H300" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I300" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J300" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K300" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L300" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M300" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s">
+        <v>144</v>
+      </c>
+      <c r="B301" t="s">
+        <v>0</v>
+      </c>
+      <c r="C301" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D301" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E301" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F301" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G301" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H301" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I301" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J301" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K301" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L301" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M301" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s">
+        <v>145</v>
+      </c>
+      <c r="B302" t="s">
+        <v>0</v>
+      </c>
+      <c r="C302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D302" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F302" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G302" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H302" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I302" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J302" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M302" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="s">
+        <v>145</v>
+      </c>
+      <c r="B303" t="s">
+        <v>0</v>
+      </c>
+      <c r="C303" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D303" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E303" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F303" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G303" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H303" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I303" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J303" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K303" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L303" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M303" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="s">
+        <v>145</v>
+      </c>
+      <c r="B304" t="s">
+        <v>0</v>
+      </c>
+      <c r="C304" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D304" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E304" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F304" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G304" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H304" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I304" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J304" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K304" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L304" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M304" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="s">
+        <v>146</v>
+      </c>
+      <c r="B305" t="s">
+        <v>0</v>
+      </c>
+      <c r="C305" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D305" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E305" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F305" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G305" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H305" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I305" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J305" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K305" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L305" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M305" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="s">
+        <v>146</v>
+      </c>
+      <c r="B306" t="s">
+        <v>0</v>
+      </c>
+      <c r="C306" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D306" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E306" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F306" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G306" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H306" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I306" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J306" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K306" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L306" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M306" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="s">
+        <v>146</v>
+      </c>
+      <c r="B307" t="s">
+        <v>0</v>
+      </c>
+      <c r="C307" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D307" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E307" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F307" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G307" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H307" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I307" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J307" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K307" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L307" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M307" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="s">
+        <v>147</v>
+      </c>
+      <c r="B308" t="s">
+        <v>0</v>
+      </c>
+      <c r="C308" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D308" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E308" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F308" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G308" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H308" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I308" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J308" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K308" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L308" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M308" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="s">
+        <v>147</v>
+      </c>
+      <c r="B309" t="s">
+        <v>0</v>
+      </c>
+      <c r="C309" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D309" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E309" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F309" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G309" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H309" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I309" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J309" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K309" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L309" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M309" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="s">
+        <v>147</v>
+      </c>
+      <c r="B310" t="s">
+        <v>0</v>
+      </c>
+      <c r="C310" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D310" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E310" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F310" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G310" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H310" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I310" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J310" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K310" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L310" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M310" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="s">
+        <v>148</v>
+      </c>
+      <c r="B311" t="s">
+        <v>0</v>
+      </c>
+      <c r="C311" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D311" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E311" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F311" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G311" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H311" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I311" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J311" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K311" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L311" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M311" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="s">
+        <v>148</v>
+      </c>
+      <c r="B312" t="s">
+        <v>0</v>
+      </c>
+      <c r="C312" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D312" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E312" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F312" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G312" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H312" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I312" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J312" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K312" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L312" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M312" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="s">
+        <v>148</v>
+      </c>
+      <c r="B313" t="s">
+        <v>0</v>
+      </c>
+      <c r="C313" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D313" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E313" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F313" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G313" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H313" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I313" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J313" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K313" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L313" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M313" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="s">
+        <v>149</v>
+      </c>
+      <c r="B314" t="s">
+        <v>0</v>
+      </c>
+      <c r="C314" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D314" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E314" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F314" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G314" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H314" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I314" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J314" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K314" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L314" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M314" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="s">
+        <v>149</v>
+      </c>
+      <c r="B315" t="s">
+        <v>0</v>
+      </c>
+      <c r="C315" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D315" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E315" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F315" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G315" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H315" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I315" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J315" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K315" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L315" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M315" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="s">
+        <v>149</v>
+      </c>
+      <c r="B316" t="s">
+        <v>0</v>
+      </c>
+      <c r="C316" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D316" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E316" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F316" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G316" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H316" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I316" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J316" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K316" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L316" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M316" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="s">
+        <v>150</v>
+      </c>
+      <c r="B317" t="s">
+        <v>0</v>
+      </c>
+      <c r="C317" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D317" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E317" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F317" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G317" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H317" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I317" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J317" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K317" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L317" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M317" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="s">
+        <v>150</v>
+      </c>
+      <c r="B318" t="s">
+        <v>0</v>
+      </c>
+      <c r="C318" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D318" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E318" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F318" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G318" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H318" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I318" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J318" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K318" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L318" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M318" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="s">
+        <v>150</v>
+      </c>
+      <c r="B319" t="s">
+        <v>0</v>
+      </c>
+      <c r="C319" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D319" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E319" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F319" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G319" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H319" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I319" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J319" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K319" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L319" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M319" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="s">
+        <v>151</v>
+      </c>
+      <c r="B320" t="s">
+        <v>0</v>
+      </c>
+      <c r="C320" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D320" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E320" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F320" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G320" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H320" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I320" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J320" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K320" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L320" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M320" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="s">
+        <v>151</v>
+      </c>
+      <c r="B321" t="s">
+        <v>0</v>
+      </c>
+      <c r="C321" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D321" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E321" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F321" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G321" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H321" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I321" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J321" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K321" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L321" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M321" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="s">
+        <v>151</v>
+      </c>
+      <c r="B322" t="s">
+        <v>0</v>
+      </c>
+      <c r="C322" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D322" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E322" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F322" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G322" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H322" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I322" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J322" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K322" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L322" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M322" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="s">
+        <v>152</v>
+      </c>
+      <c r="B323" t="s">
+        <v>0</v>
+      </c>
+      <c r="C323" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D323" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E323" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F323" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G323" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H323" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I323" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J323" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K323" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L323" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M323" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="s">
+        <v>152</v>
+      </c>
+      <c r="B324" t="s">
+        <v>0</v>
+      </c>
+      <c r="C324" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D324" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E324" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F324" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G324" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H324" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I324" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J324" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K324" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L324" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M324" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="s">
+        <v>152</v>
+      </c>
+      <c r="B325" t="s">
+        <v>0</v>
+      </c>
+      <c r="C325" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D325" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E325" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F325" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G325" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H325" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I325" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J325" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K325" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L325" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M325" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="s">
+        <v>153</v>
+      </c>
+      <c r="B326" t="s">
+        <v>0</v>
+      </c>
+      <c r="C326" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D326" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E326" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F326" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G326" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H326" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I326" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J326" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K326" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L326" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M326" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="s">
+        <v>153</v>
+      </c>
+      <c r="B327" t="s">
+        <v>0</v>
+      </c>
+      <c r="C327" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D327" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E327" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F327" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G327" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H327" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I327" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J327" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K327" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L327" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M327" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="s">
+        <v>153</v>
+      </c>
+      <c r="B328" t="s">
+        <v>0</v>
+      </c>
+      <c r="C328" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D328" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E328" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F328" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G328" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H328" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I328" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J328" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K328" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L328" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M328" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="s">
+        <v>154</v>
+      </c>
+      <c r="B329" t="s">
+        <v>0</v>
+      </c>
+      <c r="C329" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D329" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E329" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F329" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G329" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H329" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I329" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J329" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K329" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L329" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M329" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="s">
+        <v>154</v>
+      </c>
+      <c r="B330" t="s">
+        <v>0</v>
+      </c>
+      <c r="C330" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D330" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E330" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F330" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G330" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H330" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I330" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J330" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K330" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L330" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M330" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="s">
+        <v>154</v>
+      </c>
+      <c r="B331" t="s">
+        <v>0</v>
+      </c>
+      <c r="C331" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D331" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E331" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F331" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G331" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H331" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I331" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J331" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K331" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L331" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M331" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="s">
+        <v>155</v>
+      </c>
+      <c r="B332" t="s">
+        <v>0</v>
+      </c>
+      <c r="C332" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D332" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E332" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F332" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G332" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H332" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I332" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J332" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K332" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L332" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M332" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="s">
+        <v>155</v>
+      </c>
+      <c r="B333" t="s">
+        <v>0</v>
+      </c>
+      <c r="C333" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D333" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E333" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F333" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G333" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H333" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I333" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J333" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K333" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L333" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M333" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="s">
+        <v>155</v>
+      </c>
+      <c r="B334" t="s">
+        <v>0</v>
+      </c>
+      <c r="C334" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D334" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E334" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F334" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G334" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H334" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I334" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J334" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K334" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L334" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M334" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="s">
+        <v>156</v>
+      </c>
+      <c r="B335" t="s">
+        <v>0</v>
+      </c>
+      <c r="C335" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D335" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E335" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F335" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G335" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H335" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I335" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J335" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K335" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L335" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M335" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="s">
+        <v>156</v>
+      </c>
+      <c r="B336" t="s">
+        <v>0</v>
+      </c>
+      <c r="C336" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D336" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E336" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F336" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G336" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H336" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I336" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J336" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K336" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L336" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M336" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="s">
+        <v>156</v>
+      </c>
+      <c r="B337" t="s">
+        <v>0</v>
+      </c>
+      <c r="C337" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D337" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E337" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F337" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G337" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H337" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I337" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J337" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K337" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L337" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M337" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="s">
+        <v>157</v>
+      </c>
+      <c r="B338" t="s">
+        <v>0</v>
+      </c>
+      <c r="C338" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D338" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E338" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F338" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G338" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H338" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I338" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J338" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K338" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L338" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M338" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="s">
+        <v>157</v>
+      </c>
+      <c r="B339" t="s">
+        <v>0</v>
+      </c>
+      <c r="C339" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D339" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E339" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F339" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G339" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H339" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I339" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J339" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K339" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L339" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M339" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="s">
+        <v>157</v>
+      </c>
+      <c r="B340" t="s">
+        <v>0</v>
+      </c>
+      <c r="C340" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D340" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E340" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F340" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G340" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H340" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I340" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J340" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K340" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L340" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M340" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- migrate ha autodiscovery twig to POJO model
</commit_message>
<xml_diff>
--- a/data/sheet/msg_41473.xlsx
+++ b/data/sheet/msg_41473.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2101" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2131" uniqueCount="161">
   <si>
     <t/>
   </si>
@@ -503,6 +503,9 @@
   <si>
     <t>2022-03-21 13:47:36</t>
   </si>
+  <si>
+    <t>2022-03-21 17:09:29</t>
+  </si>
 </sst>
 </file>
 
@@ -854,7 +857,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I116"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4229,6 +4232,35 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>160</v>
+      </c>
+      <c r="B117" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117" t="s">
+        <v>11</v>
+      </c>
+      <c r="D117" t="n">
+        <v>1.647878972E9</v>
+      </c>
+      <c r="E117" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F117" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G117" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I117" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4236,7 +4268,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X116"/>
+  <dimension ref="A1:X117"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0"/>
   </sheetViews>
@@ -12831,6 +12863,80 @@
         <v>0</v>
       </c>
     </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>160</v>
+      </c>
+      <c r="B117" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D117" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="E117" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I117" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J117" t="n">
+        <v>1.647878971E9</v>
+      </c>
+      <c r="K117" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="L117" t="s">
+        <v>0</v>
+      </c>
+      <c r="M117" t="s">
+        <v>0</v>
+      </c>
+      <c r="N117" t="s">
+        <v>0</v>
+      </c>
+      <c r="O117" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X117" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12838,7 +12944,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M346"/>
+  <dimension ref="A1:M349"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A278" sqref="A278:XFD280"/>
@@ -27036,6 +27142,129 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="347">
+      <c r="A347" t="s">
+        <v>160</v>
+      </c>
+      <c r="B347" t="s">
+        <v>0</v>
+      </c>
+      <c r="C347" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D347" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E347" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F347" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G347" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H347" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I347" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J347" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K347" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L347" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M347" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="s">
+        <v>160</v>
+      </c>
+      <c r="B348" t="s">
+        <v>0</v>
+      </c>
+      <c r="C348" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D348" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E348" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F348" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G348" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H348" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I348" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J348" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K348" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L348" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M348" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="s">
+        <v>160</v>
+      </c>
+      <c r="B349" t="s">
+        <v>0</v>
+      </c>
+      <c r="C349" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D349" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E349" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F349" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G349" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H349" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I349" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J349" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K349" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L349" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M349" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- support for new msgId 8717
</commit_message>
<xml_diff>
--- a/data/sheet/msg_41473.xlsx
+++ b/data/sheet/msg_41473.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3031" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3121" uniqueCount="194">
   <si>
     <t/>
   </si>
@@ -596,6 +596,15 @@
   <si>
     <t>2022-03-22 12:42:11</t>
   </si>
+  <si>
+    <t>2022-03-22 13:07:03</t>
+  </si>
+  <si>
+    <t>2022-03-22 20:19:27</t>
+  </si>
+  <si>
+    <t>2022-03-23 23:36:21</t>
+  </si>
 </sst>
 </file>
 
@@ -947,7 +956,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I147"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5221,6 +5230,93 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>191</v>
+      </c>
+      <c r="B148" t="s">
+        <v>0</v>
+      </c>
+      <c r="C148" t="s">
+        <v>11</v>
+      </c>
+      <c r="D148" t="n">
+        <v>1.647950825E9</v>
+      </c>
+      <c r="E148" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F148" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G148" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H148" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I148" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>192</v>
+      </c>
+      <c r="B149" t="s">
+        <v>0</v>
+      </c>
+      <c r="C149" t="s">
+        <v>11</v>
+      </c>
+      <c r="D149" t="n">
+        <v>1.64797677E9</v>
+      </c>
+      <c r="E149" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F149" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G149" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I149" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>193</v>
+      </c>
+      <c r="B150" t="s">
+        <v>0</v>
+      </c>
+      <c r="C150" t="s">
+        <v>11</v>
+      </c>
+      <c r="D150" t="n">
+        <v>1.648074985E9</v>
+      </c>
+      <c r="E150" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F150" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G150" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I150" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5228,7 +5324,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X147"/>
+  <dimension ref="A1:X150"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0"/>
   </sheetViews>
@@ -16117,6 +16213,228 @@
         <v>0</v>
       </c>
     </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>191</v>
+      </c>
+      <c r="B148" t="s">
+        <v>0</v>
+      </c>
+      <c r="C148" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D148" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="E148" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F148" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G148" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H148" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I148" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J148" t="n">
+        <v>1.647950782E9</v>
+      </c>
+      <c r="K148" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="L148" t="s">
+        <v>0</v>
+      </c>
+      <c r="M148" t="s">
+        <v>45</v>
+      </c>
+      <c r="N148" t="s">
+        <v>0</v>
+      </c>
+      <c r="O148" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P148" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q148" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R148" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S148" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T148" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U148" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V148" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W148" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X148" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>192</v>
+      </c>
+      <c r="B149" t="s">
+        <v>0</v>
+      </c>
+      <c r="C149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D149" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="E149" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I149" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J149" t="n">
+        <v>1.647976736E9</v>
+      </c>
+      <c r="K149" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="L149" t="s">
+        <v>0</v>
+      </c>
+      <c r="M149" t="s">
+        <v>45</v>
+      </c>
+      <c r="N149" t="s">
+        <v>0</v>
+      </c>
+      <c r="O149" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X149" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>193</v>
+      </c>
+      <c r="B150" t="s">
+        <v>0</v>
+      </c>
+      <c r="C150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D150" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="E150" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G150" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H150" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I150" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J150" t="n">
+        <v>1.648074946E9</v>
+      </c>
+      <c r="K150" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="L150" t="s">
+        <v>0</v>
+      </c>
+      <c r="M150" t="s">
+        <v>45</v>
+      </c>
+      <c r="N150" t="s">
+        <v>0</v>
+      </c>
+      <c r="O150" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X150" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16124,7 +16442,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M439"/>
+  <dimension ref="A1:M448"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A278" sqref="A278:XFD280"/>
@@ -34135,6 +34453,375 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="440">
+      <c r="A440" t="s">
+        <v>191</v>
+      </c>
+      <c r="B440" t="s">
+        <v>0</v>
+      </c>
+      <c r="C440" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D440" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E440" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F440" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G440" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H440" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I440" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J440" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K440" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L440" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M440" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="s">
+        <v>191</v>
+      </c>
+      <c r="B441" t="s">
+        <v>0</v>
+      </c>
+      <c r="C441" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D441" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E441" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F441" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G441" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H441" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I441" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J441" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K441" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L441" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M441" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="s">
+        <v>191</v>
+      </c>
+      <c r="B442" t="s">
+        <v>0</v>
+      </c>
+      <c r="C442" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D442" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E442" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F442" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G442" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H442" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I442" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J442" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K442" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L442" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M442" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="s">
+        <v>192</v>
+      </c>
+      <c r="B443" t="s">
+        <v>0</v>
+      </c>
+      <c r="C443" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D443" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E443" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F443" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G443" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H443" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I443" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J443" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K443" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L443" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M443" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="s">
+        <v>192</v>
+      </c>
+      <c r="B444" t="s">
+        <v>0</v>
+      </c>
+      <c r="C444" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D444" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E444" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F444" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G444" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H444" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I444" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J444" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K444" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L444" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M444" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="s">
+        <v>192</v>
+      </c>
+      <c r="B445" t="s">
+        <v>0</v>
+      </c>
+      <c r="C445" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D445" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E445" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F445" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G445" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H445" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I445" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J445" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K445" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L445" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M445" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="s">
+        <v>193</v>
+      </c>
+      <c r="B446" t="s">
+        <v>0</v>
+      </c>
+      <c r="C446" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D446" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E446" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F446" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G446" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H446" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I446" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J446" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K446" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L446" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M446" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="s">
+        <v>193</v>
+      </c>
+      <c r="B447" t="s">
+        <v>0</v>
+      </c>
+      <c r="C447" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D447" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E447" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F447" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G447" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H447" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I447" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J447" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K447" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L447" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M447" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="s">
+        <v>193</v>
+      </c>
+      <c r="B448" t="s">
+        <v>0</v>
+      </c>
+      <c r="C448" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D448" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E448" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F448" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G448" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H448" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I448" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J448" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K448" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L448" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M448" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- fixes in reconnection
</commit_message>
<xml_diff>
--- a/data/sheet/msg_41473.xlsx
+++ b/data/sheet/msg_41473.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4201" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4231" uniqueCount="231">
   <si>
     <t/>
   </si>
@@ -713,6 +713,9 @@
   <si>
     <t>2022-07-01 17:38:09</t>
   </si>
+  <si>
+    <t>2022-07-02 13:54:44</t>
+  </si>
 </sst>
 </file>
 
@@ -1064,7 +1067,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I186"/>
+  <dimension ref="A1:I187"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6469,6 +6472,35 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>230</v>
+      </c>
+      <c r="B187" t="s">
+        <v>0</v>
+      </c>
+      <c r="C187" t="s">
+        <v>11</v>
+      </c>
+      <c r="D187" t="n">
+        <v>1.656762885E9</v>
+      </c>
+      <c r="E187" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F187" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G187" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H187" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I187" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6476,7 +6508,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X186"/>
+  <dimension ref="A1:X187"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0"/>
   </sheetViews>
@@ -20251,6 +20283,80 @@
         <v>0</v>
       </c>
     </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>230</v>
+      </c>
+      <c r="B187" t="s">
+        <v>0</v>
+      </c>
+      <c r="C187" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D187" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="E187" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F187" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G187" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H187" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I187" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J187" t="n">
+        <v>1.656762867E9</v>
+      </c>
+      <c r="K187" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="L187" t="s">
+        <v>0</v>
+      </c>
+      <c r="M187" t="s">
+        <v>45</v>
+      </c>
+      <c r="N187" t="s">
+        <v>0</v>
+      </c>
+      <c r="O187" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P187" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q187" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R187" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S187" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T187" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U187" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V187" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W187" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X187" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20258,7 +20364,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M556"/>
+  <dimension ref="A1:M559"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A278" sqref="A278:XFD280"/>
@@ -43066,6 +43172,129 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="557">
+      <c r="A557" t="s">
+        <v>230</v>
+      </c>
+      <c r="B557" t="s">
+        <v>0</v>
+      </c>
+      <c r="C557" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D557" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E557" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F557" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G557" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H557" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I557" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J557" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K557" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L557" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M557" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="s">
+        <v>230</v>
+      </c>
+      <c r="B558" t="s">
+        <v>0</v>
+      </c>
+      <c r="C558" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D558" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E558" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F558" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G558" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H558" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I558" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J558" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K558" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L558" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M558" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="s">
+        <v>230</v>
+      </c>
+      <c r="B559" t="s">
+        <v>0</v>
+      </c>
+      <c r="C559" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D559" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E559" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F559" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G559" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H559" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I559" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J559" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K559" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L559" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M559" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- architecture rebuild to fix major problems with connection lost
</commit_message>
<xml_diff>
--- a/data/sheet/msg_41473.xlsx
+++ b/data/sheet/msg_41473.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4231" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4351" uniqueCount="235">
   <si>
     <t/>
   </si>
@@ -716,6 +716,18 @@
   <si>
     <t>2022-07-02 13:54:44</t>
   </si>
+  <si>
+    <t>2022-07-04 21:08:40</t>
+  </si>
+  <si>
+    <t>2022-07-05 10:47:52</t>
+  </si>
+  <si>
+    <t>2022-07-05 11:38:52</t>
+  </si>
+  <si>
+    <t>2022-07-05 18:08:15</t>
+  </si>
 </sst>
 </file>
 
@@ -1067,7 +1079,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I187"/>
+  <dimension ref="A1:I191"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6501,6 +6513,122 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>231</v>
+      </c>
+      <c r="B188" t="s">
+        <v>0</v>
+      </c>
+      <c r="C188" t="s">
+        <v>11</v>
+      </c>
+      <c r="D188" t="n">
+        <v>1.656961723E9</v>
+      </c>
+      <c r="E188" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F188" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G188" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H188" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I188" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>232</v>
+      </c>
+      <c r="B189" t="s">
+        <v>0</v>
+      </c>
+      <c r="C189" t="s">
+        <v>11</v>
+      </c>
+      <c r="D189" t="n">
+        <v>1.657010878E9</v>
+      </c>
+      <c r="E189" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F189" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G189" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H189" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I189" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>233</v>
+      </c>
+      <c r="B190" t="s">
+        <v>0</v>
+      </c>
+      <c r="C190" t="s">
+        <v>11</v>
+      </c>
+      <c r="D190" t="n">
+        <v>1.657013938E9</v>
+      </c>
+      <c r="E190" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F190" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G190" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I190" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>234</v>
+      </c>
+      <c r="B191" t="s">
+        <v>0</v>
+      </c>
+      <c r="C191" t="s">
+        <v>11</v>
+      </c>
+      <c r="D191" t="n">
+        <v>1.657037303E9</v>
+      </c>
+      <c r="E191" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F191" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G191" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H191" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I191" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6508,7 +6636,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X187"/>
+  <dimension ref="A1:X191"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0"/>
   </sheetViews>
@@ -20357,6 +20485,302 @@
         <v>0</v>
       </c>
     </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>231</v>
+      </c>
+      <c r="B188" t="s">
+        <v>0</v>
+      </c>
+      <c r="C188" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D188" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="E188" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F188" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G188" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H188" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I188" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J188" t="n">
+        <v>1.656961667E9</v>
+      </c>
+      <c r="K188" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="L188" t="s">
+        <v>0</v>
+      </c>
+      <c r="M188" t="s">
+        <v>45</v>
+      </c>
+      <c r="N188" t="s">
+        <v>0</v>
+      </c>
+      <c r="O188" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P188" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q188" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R188" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S188" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T188" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U188" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V188" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W188" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X188" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>232</v>
+      </c>
+      <c r="B189" t="s">
+        <v>0</v>
+      </c>
+      <c r="C189" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D189" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="E189" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F189" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G189" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H189" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I189" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J189" t="n">
+        <v>1.657010831E9</v>
+      </c>
+      <c r="K189" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="L189" t="s">
+        <v>0</v>
+      </c>
+      <c r="M189" t="s">
+        <v>45</v>
+      </c>
+      <c r="N189" t="s">
+        <v>0</v>
+      </c>
+      <c r="O189" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P189" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q189" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R189" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S189" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T189" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U189" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V189" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W189" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X189" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>233</v>
+      </c>
+      <c r="B190" t="s">
+        <v>0</v>
+      </c>
+      <c r="C190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D190" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="E190" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I190" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J190" t="n">
+        <v>1.657013925E9</v>
+      </c>
+      <c r="K190" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="L190" t="s">
+        <v>0</v>
+      </c>
+      <c r="M190" t="s">
+        <v>45</v>
+      </c>
+      <c r="N190" t="s">
+        <v>0</v>
+      </c>
+      <c r="O190" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W190" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X190" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>234</v>
+      </c>
+      <c r="B191" t="s">
+        <v>0</v>
+      </c>
+      <c r="C191" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D191" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="E191" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F191" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G191" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="H191" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="I191" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J191" t="n">
+        <v>1.657037247E9</v>
+      </c>
+      <c r="K191" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="L191" t="s">
+        <v>0</v>
+      </c>
+      <c r="M191" t="s">
+        <v>45</v>
+      </c>
+      <c r="N191" t="s">
+        <v>0</v>
+      </c>
+      <c r="O191" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P191" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q191" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R191" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S191" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T191" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U191" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V191" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W191" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X191" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20364,7 +20788,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M559"/>
+  <dimension ref="A1:M571"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A278" sqref="A278:XFD280"/>
@@ -43295,6 +43719,498 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="560">
+      <c r="A560" t="s">
+        <v>231</v>
+      </c>
+      <c r="B560" t="s">
+        <v>0</v>
+      </c>
+      <c r="C560" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D560" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E560" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F560" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G560" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H560" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I560" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J560" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K560" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L560" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M560" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="s">
+        <v>231</v>
+      </c>
+      <c r="B561" t="s">
+        <v>0</v>
+      </c>
+      <c r="C561" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D561" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E561" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F561" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G561" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H561" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I561" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J561" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K561" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L561" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M561" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="s">
+        <v>231</v>
+      </c>
+      <c r="B562" t="s">
+        <v>0</v>
+      </c>
+      <c r="C562" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D562" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E562" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F562" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G562" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H562" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I562" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J562" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K562" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L562" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M562" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="s">
+        <v>232</v>
+      </c>
+      <c r="B563" t="s">
+        <v>0</v>
+      </c>
+      <c r="C563" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D563" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E563" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F563" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G563" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H563" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I563" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J563" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K563" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L563" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M563" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="s">
+        <v>232</v>
+      </c>
+      <c r="B564" t="s">
+        <v>0</v>
+      </c>
+      <c r="C564" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D564" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E564" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F564" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G564" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H564" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I564" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J564" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K564" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L564" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M564" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="s">
+        <v>232</v>
+      </c>
+      <c r="B565" t="s">
+        <v>0</v>
+      </c>
+      <c r="C565" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D565" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E565" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F565" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G565" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H565" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I565" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J565" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K565" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L565" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M565" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="s">
+        <v>233</v>
+      </c>
+      <c r="B566" t="s">
+        <v>0</v>
+      </c>
+      <c r="C566" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D566" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E566" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F566" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G566" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H566" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I566" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J566" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K566" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L566" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M566" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="s">
+        <v>233</v>
+      </c>
+      <c r="B567" t="s">
+        <v>0</v>
+      </c>
+      <c r="C567" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D567" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E567" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F567" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G567" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H567" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I567" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J567" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K567" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L567" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M567" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="s">
+        <v>233</v>
+      </c>
+      <c r="B568" t="s">
+        <v>0</v>
+      </c>
+      <c r="C568" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D568" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E568" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F568" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G568" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H568" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I568" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J568" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K568" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L568" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M568" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="s">
+        <v>234</v>
+      </c>
+      <c r="B569" t="s">
+        <v>0</v>
+      </c>
+      <c r="C569" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D569" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E569" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F569" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G569" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H569" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I569" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J569" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K569" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L569" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M569" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="s">
+        <v>234</v>
+      </c>
+      <c r="B570" t="s">
+        <v>0</v>
+      </c>
+      <c r="C570" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D570" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E570" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F570" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G570" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H570" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I570" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J570" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K570" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L570" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M570" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="s">
+        <v>234</v>
+      </c>
+      <c r="B571" t="s">
+        <v>0</v>
+      </c>
+      <c r="C571" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D571" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E571" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F571" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G571" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H571" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I571" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="J571" t="n">
+        <v>8193.0</v>
+      </c>
+      <c r="K571" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L571" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M571" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- hotfix in start script
</commit_message>
<xml_diff>
--- a/data/sheet/msg_41473.xlsx
+++ b/data/sheet/msg_41473.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4351" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4393" uniqueCount="236">
   <si>
     <t/>
   </si>
@@ -728,6 +728,9 @@
   <si>
     <t>2022-07-05 18:08:15</t>
   </si>
+  <si>
+    <t>2022-10-27 20:27:14</t>
+  </si>
 </sst>
 </file>
 
@@ -1079,7 +1082,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I191"/>
+  <dimension ref="A1:I192"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6629,6 +6632,35 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>235</v>
+      </c>
+      <c r="B192" t="s">
+        <v>0</v>
+      </c>
+      <c r="C192" t="s">
+        <v>11</v>
+      </c>
+      <c r="D192" t="n">
+        <v>1.666895238E9</v>
+      </c>
+      <c r="E192" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F192" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="G192" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H192" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I192" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6636,7 +6668,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X191"/>
+  <dimension ref="A1:X192"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0"/>
   </sheetViews>
@@ -20781,6 +20813,80 @@
         <v>0</v>
       </c>
     </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>235</v>
+      </c>
+      <c r="B192" t="s">
+        <v>0</v>
+      </c>
+      <c r="C192" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D192" t="n">
+        <v>527.0</v>
+      </c>
+      <c r="E192" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="F192" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G192" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="H192" t="n">
+        <v>160.0</v>
+      </c>
+      <c r="I192" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J192" t="n">
+        <v>1.66689481E9</v>
+      </c>
+      <c r="K192" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="L192" t="s">
+        <v>0</v>
+      </c>
+      <c r="M192" t="s">
+        <v>45</v>
+      </c>
+      <c r="N192" t="s">
+        <v>0</v>
+      </c>
+      <c r="O192" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="P192" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q192" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R192" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S192" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T192" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U192" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V192" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W192" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X192" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20788,7 +20894,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M571"/>
+  <dimension ref="A1:M577"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A278" sqref="A278:XFD280"/>
@@ -44211,6 +44317,252 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="572">
+      <c r="A572" t="s">
+        <v>235</v>
+      </c>
+      <c r="B572" t="s">
+        <v>0</v>
+      </c>
+      <c r="C572" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D572" t="n">
+        <v>1.9110224228993E13</v>
+      </c>
+      <c r="E572" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F572" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G572" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H572" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I572" t="n">
+        <v>10752.0</v>
+      </c>
+      <c r="J572" t="n">
+        <v>8192.0</v>
+      </c>
+      <c r="K572" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L572" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M572" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="s">
+        <v>235</v>
+      </c>
+      <c r="B573" t="s">
+        <v>0</v>
+      </c>
+      <c r="C573" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D573" t="n">
+        <v>1.9110224226576E13</v>
+      </c>
+      <c r="E573" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F573" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G573" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H573" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I573" t="n">
+        <v>10752.0</v>
+      </c>
+      <c r="J573" t="n">
+        <v>8192.0</v>
+      </c>
+      <c r="K573" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L573" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M573" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="s">
+        <v>235</v>
+      </c>
+      <c r="B574" t="s">
+        <v>0</v>
+      </c>
+      <c r="C574" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D574" t="n">
+        <v>1.9110224228646E13</v>
+      </c>
+      <c r="E574" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F574" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="G574" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="H574" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I574" t="n">
+        <v>10752.0</v>
+      </c>
+      <c r="J574" t="n">
+        <v>8192.0</v>
+      </c>
+      <c r="K574" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L574" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M574" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="s">
+        <v>235</v>
+      </c>
+      <c r="B575" t="s">
+        <v>0</v>
+      </c>
+      <c r="C575" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D575" t="n">
+        <v>1.9110459090465E13</v>
+      </c>
+      <c r="E575" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F575" t="n">
+        <v>10016.0</v>
+      </c>
+      <c r="G575" t="n">
+        <v>2.69627393E8</v>
+      </c>
+      <c r="H575" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I575" t="n">
+        <v>10752.0</v>
+      </c>
+      <c r="J575" t="n">
+        <v>8192.0</v>
+      </c>
+      <c r="K575" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L575" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M575" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="s">
+        <v>235</v>
+      </c>
+      <c r="B576" t="s">
+        <v>0</v>
+      </c>
+      <c r="C576" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D576" t="n">
+        <v>1.9110459090976E13</v>
+      </c>
+      <c r="E576" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F576" t="n">
+        <v>10016.0</v>
+      </c>
+      <c r="G576" t="n">
+        <v>2.69627393E8</v>
+      </c>
+      <c r="H576" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I576" t="n">
+        <v>10752.0</v>
+      </c>
+      <c r="J576" t="n">
+        <v>8192.0</v>
+      </c>
+      <c r="K576" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L576" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M576" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="s">
+        <v>235</v>
+      </c>
+      <c r="B577" t="s">
+        <v>0</v>
+      </c>
+      <c r="C577" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D577" t="n">
+        <v>1.9110459093129E13</v>
+      </c>
+      <c r="E577" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F577" t="n">
+        <v>10016.0</v>
+      </c>
+      <c r="G577" t="n">
+        <v>2.69627393E8</v>
+      </c>
+      <c r="H577" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="I577" t="n">
+        <v>10752.0</v>
+      </c>
+      <c r="J577" t="n">
+        <v>8192.0</v>
+      </c>
+      <c r="K577" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L577" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M577" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>